<commit_message>
make risklist for iteration 6
</commit_message>
<xml_diff>
--- a/docs/project_management/resources/Risklist.xlsx
+++ b/docs/project_management/resources/Risklist.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
   <si>
     <t>Iteration</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>Cross-train team members to mitigate the impact</t>
+  </si>
+  <si>
+    <t>Ø</t>
   </si>
 </sst>
 </file>
@@ -297,7 +300,7 @@
     <numFmt numFmtId="164" formatCode="d.m.yyyy"/>
     <numFmt numFmtId="165" formatCode="dd.mm.yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -325,6 +328,12 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -347,12 +356,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF6AA84F"/>
         <bgColor rgb="FF6AA84F"/>
       </patternFill>
@@ -363,14 +366,62 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -378,14 +429,12 @@
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -400,14 +449,40 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -653,6 +728,7 @@
     <col customWidth="1" min="4" max="4" width="39.63"/>
     <col customWidth="1" min="5" max="5" width="35.88"/>
     <col customWidth="1" min="6" max="6" width="9.38"/>
+    <col customWidth="1" min="7" max="7" width="19.75"/>
     <col customWidth="1" min="8" max="8" width="4.0"/>
     <col customWidth="1" min="9" max="9" width="4.5"/>
     <col customWidth="1" min="10" max="10" width="4.88"/>
@@ -664,6 +740,14 @@
     <col customWidth="1" min="16" max="16" width="4.75"/>
     <col customWidth="1" min="17" max="17" width="4.5"/>
     <col customWidth="1" min="18" max="18" width="4.88"/>
+    <col customWidth="1" min="19" max="19" width="5.25"/>
+    <col customWidth="1" min="20" max="20" width="4.88"/>
+    <col customWidth="1" min="21" max="21" width="4.5"/>
+    <col customWidth="1" min="22" max="22" width="4.88"/>
+    <col customWidth="1" min="23" max="23" width="4.5"/>
+    <col customWidth="1" min="24" max="24" width="4.88"/>
+    <col customWidth="1" min="25" max="25" width="4.5"/>
+    <col customWidth="1" min="26" max="28" width="4.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -673,1152 +757,1768 @@
       <c r="I1" s="2">
         <v>1.0</v>
       </c>
-      <c r="J1" s="3"/>
       <c r="K1" s="2">
         <v>2.0</v>
       </c>
-      <c r="L1" s="3"/>
       <c r="M1" s="2">
         <v>3.0</v>
       </c>
-      <c r="N1" s="3"/>
       <c r="O1" s="2">
         <v>4.0</v>
       </c>
-      <c r="P1" s="3"/>
       <c r="Q1" s="2">
         <v>5.0</v>
       </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
+      <c r="S1" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="U1" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="W1" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="Y1" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
+      <c r="S2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>1.0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="7">
         <v>45243.0</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="9">
         <v>5.0</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="10">
         <v>0.8</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="11">
         <f t="shared" ref="J3:J20" si="1">H3*I3</f>
         <v>4</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="10">
         <v>0.6</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="11">
         <f t="shared" ref="L3:L20" si="2">H3*K3</f>
         <v>3</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="10">
         <v>0.2</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="11">
         <f t="shared" ref="N3:N20" si="3">H3*M3</f>
         <v>1</v>
       </c>
-      <c r="O3" s="11">
+      <c r="O3" s="10">
         <v>0.1</v>
       </c>
-      <c r="P3" s="10">
+      <c r="P3" s="11">
         <f t="shared" ref="P3:P20" si="4">H3*O3</f>
         <v>0.5</v>
       </c>
-      <c r="Q3" s="11">
+      <c r="Q3" s="10">
         <v>0.05</v>
       </c>
-      <c r="R3" s="10">
+      <c r="R3" s="11">
         <f t="shared" ref="R3:R20" si="5">H3*Q3</f>
         <v>0.25</v>
       </c>
+      <c r="S3" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="T3" s="11">
+        <f t="shared" ref="T3:T20" si="6">H3*S3</f>
+        <v>0.1</v>
+      </c>
+      <c r="U3" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V3" s="11">
+        <f t="shared" ref="V3:V20" si="7">H3*U3</f>
+        <v>0</v>
+      </c>
+      <c r="W3" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X3" s="11">
+        <f t="shared" ref="X3:X20" si="8">H3*W3</f>
+        <v>0</v>
+      </c>
+      <c r="Y3" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z3" s="11">
+        <f t="shared" ref="Z3:Z20" si="9">H3*Y3</f>
+        <v>0</v>
+      </c>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>2.0</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>45243.0</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="9">
         <v>4.0</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="13">
         <v>0.7</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="14">
         <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="13">
         <v>0.5</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="14">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="13">
         <v>0.25</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="14">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="13">
         <v>0.2</v>
       </c>
-      <c r="P4" s="10">
+      <c r="P4" s="14">
         <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="Q4" s="11">
+      <c r="Q4" s="13">
         <v>0.07</v>
       </c>
-      <c r="R4" s="10">
+      <c r="R4" s="14">
         <f t="shared" si="5"/>
         <v>0.28</v>
       </c>
+      <c r="S4" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="T4" s="14">
+        <f t="shared" si="6"/>
+        <v>0.2</v>
+      </c>
+      <c r="U4" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V4" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W4" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X4" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y4" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z4" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>3.0</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>45243.0</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="9">
         <v>3.0</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="13">
         <v>0.6</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="14">
         <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="13">
         <v>0.3</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="14">
         <f t="shared" si="2"/>
         <v>0.9</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="13">
         <v>0.15</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="14">
         <f t="shared" si="3"/>
         <v>0.45</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="13">
         <v>0.1</v>
       </c>
-      <c r="P5" s="10">
+      <c r="P5" s="14">
         <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
-      <c r="Q5" s="11">
+      <c r="Q5" s="13">
         <v>0.05</v>
       </c>
-      <c r="R5" s="10">
+      <c r="R5" s="14">
         <f t="shared" si="5"/>
         <v>0.15</v>
       </c>
+      <c r="S5" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="T5" s="14">
+        <f t="shared" si="6"/>
+        <v>0.06</v>
+      </c>
+      <c r="U5" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V5" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W5" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X5" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y5" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z5" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>4.0</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>45243.0</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="9">
         <v>5.0</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="13">
         <v>0.8</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="13">
         <v>0.5</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="14">
         <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="13">
         <v>0.1</v>
       </c>
-      <c r="N6" s="10">
+      <c r="N6" s="14">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="13">
         <v>0.05</v>
       </c>
-      <c r="P6" s="10">
+      <c r="P6" s="14">
         <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
-      <c r="Q6" s="11">
+      <c r="Q6" s="13">
         <v>0.02</v>
       </c>
-      <c r="R6" s="10">
+      <c r="R6" s="14">
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
+      <c r="S6" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="T6" s="14">
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="U6" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V6" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X6" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z6" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>5.0</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <v>45250.0</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="9">
         <v>4.0</v>
       </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="10">
+      <c r="I7" s="15"/>
+      <c r="J7" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="13">
         <v>0.8</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="14">
         <f t="shared" si="2"/>
         <v>3.2</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="13">
         <v>0.4</v>
       </c>
-      <c r="N7" s="10">
+      <c r="N7" s="14">
         <f t="shared" si="3"/>
         <v>1.6</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="13">
         <v>0.2</v>
       </c>
-      <c r="P7" s="10">
+      <c r="P7" s="14">
         <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="Q7" s="11">
+      <c r="Q7" s="13">
         <v>0.05</v>
       </c>
-      <c r="R7" s="10">
+      <c r="R7" s="14">
         <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
+      <c r="S7" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="T7" s="14">
+        <f t="shared" si="6"/>
+        <v>0.08</v>
+      </c>
+      <c r="U7" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V7" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W7" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X7" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z7" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
     </row>
     <row r="8">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>6.0</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>45250.0</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="9">
         <v>3.0</v>
       </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="10">
+      <c r="I8" s="15"/>
+      <c r="J8" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="13">
         <v>0.7</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="14">
         <f t="shared" si="2"/>
         <v>2.1</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="13">
         <v>0.5</v>
       </c>
-      <c r="N8" s="10">
+      <c r="N8" s="14">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="13">
         <v>0.25</v>
       </c>
-      <c r="P8" s="10">
+      <c r="P8" s="14">
         <f t="shared" si="4"/>
         <v>0.75</v>
       </c>
-      <c r="Q8" s="11">
+      <c r="Q8" s="13">
         <v>0.1</v>
       </c>
-      <c r="R8" s="10">
+      <c r="R8" s="14">
         <f t="shared" si="5"/>
         <v>0.3</v>
       </c>
+      <c r="S8" s="13">
+        <v>0.07</v>
+      </c>
+      <c r="T8" s="14">
+        <f t="shared" si="6"/>
+        <v>0.21</v>
+      </c>
+      <c r="U8" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V8" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X8" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z8" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
     </row>
     <row r="9">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>7.0</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>45250.0</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="9">
         <v>3.0</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="10">
+      <c r="I9" s="15"/>
+      <c r="J9" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="13">
         <v>0.8</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="14">
         <f t="shared" si="2"/>
         <v>2.4</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="13">
         <v>0.3</v>
       </c>
-      <c r="N9" s="10">
+      <c r="N9" s="14">
         <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="13">
         <v>0.15</v>
       </c>
-      <c r="P9" s="10">
+      <c r="P9" s="14">
         <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
-      <c r="Q9" s="11">
+      <c r="Q9" s="13">
         <v>0.07</v>
       </c>
-      <c r="R9" s="10">
+      <c r="R9" s="14">
         <f t="shared" si="5"/>
         <v>0.21</v>
       </c>
+      <c r="S9" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="T9" s="14">
+        <f t="shared" si="6"/>
+        <v>0.15</v>
+      </c>
+      <c r="U9" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V9" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W9" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X9" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z9" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
     </row>
     <row r="10">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>8.0</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <v>45257.0</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="9">
         <v>4.0</v>
       </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="10">
+      <c r="I10" s="15"/>
+      <c r="J10" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="10">
+      <c r="K10" s="15"/>
+      <c r="L10" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="13">
         <v>0.8</v>
       </c>
-      <c r="N10" s="10">
+      <c r="N10" s="14">
         <f t="shared" si="3"/>
         <v>3.2</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="13">
         <v>0.5</v>
       </c>
-      <c r="P10" s="10">
+      <c r="P10" s="14">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="Q10" s="11">
+      <c r="Q10" s="13">
         <v>0.1</v>
       </c>
-      <c r="R10" s="10">
+      <c r="R10" s="14">
         <f t="shared" si="5"/>
         <v>0.4</v>
       </c>
+      <c r="S10" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="T10" s="14">
+        <f t="shared" si="6"/>
+        <v>0.2</v>
+      </c>
+      <c r="U10" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V10" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W10" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X10" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y10" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z10" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
     </row>
     <row r="11">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <v>9.0</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <v>45258.0</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="9">
         <v>3.0</v>
       </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="10">
+      <c r="I11" s="15"/>
+      <c r="J11" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="10">
+      <c r="K11" s="15"/>
+      <c r="L11" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="13">
         <v>0.7</v>
       </c>
-      <c r="N11" s="10">
+      <c r="N11" s="14">
         <f t="shared" si="3"/>
         <v>2.1</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O11" s="13">
         <v>0.6</v>
       </c>
-      <c r="P11" s="10">
+      <c r="P11" s="14">
         <f t="shared" si="4"/>
         <v>1.8</v>
       </c>
-      <c r="Q11" s="11">
+      <c r="Q11" s="13">
         <v>0.2</v>
       </c>
-      <c r="R11" s="10">
+      <c r="R11" s="14">
         <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
+      <c r="S11" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="T11" s="14">
+        <f t="shared" si="6"/>
+        <v>0.3</v>
+      </c>
+      <c r="U11" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V11" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X11" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z11" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
     </row>
     <row r="12">
-      <c r="A12" s="6">
+      <c r="A12" s="4">
         <v>10.0</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <v>45260.0</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="9">
         <v>5.0</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="10">
+      <c r="I12" s="15"/>
+      <c r="J12" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="10">
+      <c r="K12" s="15"/>
+      <c r="L12" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="13">
         <v>0.8</v>
       </c>
-      <c r="N12" s="10">
+      <c r="N12" s="14">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="O12" s="11">
+      <c r="O12" s="13">
         <v>0.5</v>
       </c>
-      <c r="P12" s="10">
+      <c r="P12" s="14">
         <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
-      <c r="Q12" s="11">
+      <c r="Q12" s="13">
         <v>0.1</v>
       </c>
-      <c r="R12" s="10">
+      <c r="R12" s="14">
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
+      <c r="S12" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="T12" s="14">
+        <f t="shared" si="6"/>
+        <v>0.25</v>
+      </c>
+      <c r="U12" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V12" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W12" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X12" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z12" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
     </row>
     <row r="13">
-      <c r="A13" s="6">
+      <c r="A13" s="4">
         <v>11.0</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="16">
         <v>45261.0</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="9">
         <v>3.0</v>
       </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="10">
+      <c r="I13" s="15"/>
+      <c r="J13" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="10">
+      <c r="K13" s="15"/>
+      <c r="L13" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="13">
         <v>0.6</v>
       </c>
-      <c r="N13" s="10">
+      <c r="N13" s="14">
         <f t="shared" si="3"/>
         <v>1.8</v>
       </c>
-      <c r="O13" s="11">
+      <c r="O13" s="13">
         <v>0.4</v>
       </c>
-      <c r="P13" s="10">
+      <c r="P13" s="14">
         <f t="shared" si="4"/>
         <v>1.2</v>
       </c>
-      <c r="Q13" s="11">
+      <c r="Q13" s="13">
         <v>0.17</v>
       </c>
-      <c r="R13" s="10">
+      <c r="R13" s="14">
         <f t="shared" si="5"/>
         <v>0.51</v>
       </c>
+      <c r="S13" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="T13" s="14">
+        <f t="shared" si="6"/>
+        <v>0.3</v>
+      </c>
+      <c r="U13" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V13" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W13" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X13" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z13" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
     </row>
     <row r="14">
-      <c r="A14" s="6">
+      <c r="A14" s="4">
         <v>12.0</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="16">
         <v>45265.0</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="9">
         <v>4.0</v>
       </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="10">
+      <c r="I14" s="15"/>
+      <c r="J14" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K14" s="12"/>
-      <c r="L14" s="10">
+      <c r="K14" s="15"/>
+      <c r="L14" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M14" s="13">
         <v>0.7</v>
       </c>
-      <c r="N14" s="10">
+      <c r="N14" s="14">
         <f t="shared" si="3"/>
         <v>2.8</v>
       </c>
-      <c r="O14" s="11">
+      <c r="O14" s="13">
         <v>0.3</v>
       </c>
-      <c r="P14" s="10">
+      <c r="P14" s="14">
         <f t="shared" si="4"/>
         <v>1.2</v>
       </c>
-      <c r="Q14" s="11">
+      <c r="Q14" s="13">
         <v>0.15</v>
       </c>
-      <c r="R14" s="10">
+      <c r="R14" s="14">
         <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
+      <c r="S14" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="T14" s="14">
+        <f t="shared" si="6"/>
+        <v>0.4</v>
+      </c>
+      <c r="U14" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V14" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W14" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X14" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z14" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
     </row>
     <row r="15">
-      <c r="A15" s="6">
+      <c r="A15" s="4">
         <v>13.0</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <v>45271.0</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="9">
         <v>3.0</v>
       </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="10">
+      <c r="I15" s="15"/>
+      <c r="J15" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K15" s="12"/>
-      <c r="L15" s="10">
+      <c r="K15" s="15"/>
+      <c r="L15" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="13">
         <v>0.8</v>
       </c>
-      <c r="N15" s="10">
+      <c r="N15" s="14">
         <f t="shared" si="3"/>
         <v>2.4</v>
       </c>
-      <c r="O15" s="11">
+      <c r="O15" s="13">
         <v>0.5</v>
       </c>
-      <c r="P15" s="10">
+      <c r="P15" s="14">
         <f t="shared" si="4"/>
         <v>1.5</v>
       </c>
-      <c r="Q15" s="11">
+      <c r="Q15" s="13">
         <v>0.2</v>
       </c>
-      <c r="R15" s="10">
+      <c r="R15" s="14">
         <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
+      <c r="S15" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="T15" s="14">
+        <f t="shared" si="6"/>
+        <v>0.15</v>
+      </c>
+      <c r="U15" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V15" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W15" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X15" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z15" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="8"/>
     </row>
     <row r="16">
-      <c r="A16" s="6">
+      <c r="A16" s="4">
         <v>14.0</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="7">
         <v>45271.0</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="9">
         <v>4.0</v>
       </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="10">
+      <c r="I16" s="15"/>
+      <c r="J16" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K16" s="12"/>
-      <c r="L16" s="10">
+      <c r="K16" s="15"/>
+      <c r="L16" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M16" s="12"/>
-      <c r="N16" s="10">
+      <c r="M16" s="15"/>
+      <c r="N16" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="13">
         <v>0.6</v>
       </c>
-      <c r="P16" s="10">
+      <c r="P16" s="14">
         <f t="shared" si="4"/>
         <v>2.4</v>
       </c>
-      <c r="Q16" s="11">
+      <c r="Q16" s="13">
         <v>0.15</v>
       </c>
-      <c r="R16" s="10">
+      <c r="R16" s="14">
         <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
+      <c r="S16" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="T16" s="14">
+        <f t="shared" si="6"/>
+        <v>0.4</v>
+      </c>
+      <c r="U16" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V16" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W16" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X16" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z16" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA16" s="8"/>
+      <c r="AB16" s="8"/>
     </row>
     <row r="17">
-      <c r="A17" s="6">
+      <c r="A17" s="4">
         <v>15.0</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="7">
         <v>45271.0</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="9">
         <v>3.0</v>
       </c>
-      <c r="I17" s="12"/>
-      <c r="J17" s="10">
+      <c r="I17" s="15"/>
+      <c r="J17" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K17" s="12"/>
-      <c r="L17" s="10">
+      <c r="K17" s="15"/>
+      <c r="L17" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M17" s="12"/>
-      <c r="N17" s="10">
+      <c r="M17" s="15"/>
+      <c r="N17" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O17" s="11">
+      <c r="O17" s="13">
         <v>0.8</v>
       </c>
-      <c r="P17" s="10">
+      <c r="P17" s="14">
         <f t="shared" si="4"/>
         <v>2.4</v>
       </c>
-      <c r="Q17" s="11">
+      <c r="Q17" s="13">
         <v>0.3</v>
       </c>
-      <c r="R17" s="10">
+      <c r="R17" s="14">
         <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
+      <c r="S17" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="T17" s="14">
+        <f t="shared" si="6"/>
+        <v>0.6</v>
+      </c>
+      <c r="U17" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V17" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W17" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X17" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z17" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA17" s="8"/>
+      <c r="AB17" s="8"/>
     </row>
     <row r="18">
-      <c r="A18" s="6">
+      <c r="A18" s="4">
         <v>16.0</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <v>45278.0</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="9">
         <v>5.0</v>
       </c>
-      <c r="I18" s="12"/>
-      <c r="J18" s="10">
+      <c r="I18" s="15"/>
+      <c r="J18" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K18" s="12"/>
-      <c r="L18" s="10">
+      <c r="K18" s="15"/>
+      <c r="L18" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M18" s="12"/>
-      <c r="N18" s="10">
+      <c r="M18" s="15"/>
+      <c r="N18" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O18" s="11">
+      <c r="O18" s="13">
         <v>0.8</v>
       </c>
-      <c r="P18" s="10">
+      <c r="P18" s="14">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="Q18" s="11">
+      <c r="Q18" s="13">
         <v>0.1</v>
       </c>
-      <c r="R18" s="10">
+      <c r="R18" s="14">
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
+      <c r="S18" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="T18" s="14">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="U18" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V18" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W18" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X18" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z18" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA18" s="8"/>
+      <c r="AB18" s="8"/>
     </row>
     <row r="19">
-      <c r="A19" s="6">
+      <c r="A19" s="4">
         <v>17.0</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="7">
         <v>45278.0</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="9">
         <v>5.0</v>
       </c>
-      <c r="I19" s="12"/>
-      <c r="J19" s="10">
+      <c r="I19" s="15"/>
+      <c r="J19" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K19" s="12"/>
-      <c r="L19" s="10">
+      <c r="K19" s="15"/>
+      <c r="L19" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M19" s="12"/>
-      <c r="N19" s="10">
+      <c r="M19" s="15"/>
+      <c r="N19" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O19" s="11">
+      <c r="O19" s="13">
         <v>0.8</v>
       </c>
-      <c r="P19" s="10">
+      <c r="P19" s="14">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="Q19" s="11">
+      <c r="Q19" s="13">
         <v>0.2</v>
       </c>
-      <c r="R19" s="10">
+      <c r="R19" s="14">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
+      <c r="S19" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="T19" s="14">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="U19" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V19" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W19" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X19" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z19" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="8"/>
     </row>
     <row r="20">
-      <c r="A20" s="6">
+      <c r="A20" s="4">
         <v>18.0</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <v>45280.0</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="9">
         <v>5.0</v>
       </c>
-      <c r="I20" s="12"/>
-      <c r="J20" s="10">
+      <c r="I20" s="17"/>
+      <c r="J20" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K20" s="12"/>
-      <c r="L20" s="10">
+      <c r="K20" s="17"/>
+      <c r="L20" s="18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M20" s="12"/>
-      <c r="N20" s="10">
+      <c r="M20" s="17"/>
+      <c r="N20" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O20" s="12"/>
-      <c r="P20" s="10">
+      <c r="O20" s="17"/>
+      <c r="P20" s="18">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="11">
+      <c r="Q20" s="19">
         <v>0.9</v>
       </c>
-      <c r="R20" s="10">
+      <c r="R20" s="18">
         <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
+      <c r="S20" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="T20" s="18">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="U20" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="V20" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W20" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="X20" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y20" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="Z20" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="8"/>
     </row>
     <row r="21">
-      <c r="A21" s="14"/>
+      <c r="A21" s="20"/>
     </row>
     <row r="22">
-      <c r="A22" s="14"/>
+      <c r="A22" s="20"/>
+      <c r="H22" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" s="22">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ROUND(AVERAGE(FILTER(J3:J20, J3:J20&lt;&gt;0)),2)"),3.15)</f>
+        <v>3.15</v>
+      </c>
+      <c r="K22" s="22">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ROUND(AVERAGE(FILTER(L3:L20, L3:L20&lt;&gt;0)),2)"),2.3)</f>
+        <v>2.3</v>
+      </c>
+      <c r="M22" s="22">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ROUND(AVERAGE(FILTER(N3:N20, N3:N20&lt;&gt;0)),2)"),1.79)</f>
+        <v>1.79</v>
+      </c>
+      <c r="O22" s="22">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ROUND(AVERAGE(FILTER(P3:P20, P3:P20&lt;&gt;0)),2)"),1.58)</f>
+        <v>1.58</v>
+      </c>
+      <c r="Q22" s="22">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ROUND(AVERAGE(FILTER(R3:R20, R3:R20&lt;&gt;0)),2)"),0.68)</f>
+        <v>0.68</v>
+      </c>
+      <c r="S22" s="22">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ROUND(AVERAGE(FILTER(T3:T20, T3:T20&lt;&gt;0)),2)"),0.31)</f>
+        <v>0.31</v>
+      </c>
+      <c r="U22" s="22" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ROUND(AVERAGE(FILTER(V3:V20, V3:V20&lt;&gt;0)),2)"),"#N/A")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="W22" s="22" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ROUND(AVERAGE(FILTER(X3:X20, X3:X20&lt;&gt;0)),2)"),"#N/A")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y22" s="22" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ROUND(AVERAGE(FILTER(Z3:Z20, Z3:Z20&lt;&gt;0)),2)"),"#N/A")</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="14"/>
+      <c r="A23" s="20"/>
     </row>
     <row r="24">
-      <c r="A24" s="14"/>
+      <c r="A24" s="20"/>
     </row>
     <row r="25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="19">
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="Y22:Z22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:V22"/>
   </mergeCells>
-  <conditionalFormatting sqref="I3:I20 K3:K20 M3:M20 O3:O20 Q3:Q20">
+  <conditionalFormatting sqref="I3:I20 K3:K20 M3:M20 O3:O20 Q3:Q20 S3:S20 U3:U20 W3:W20 Y3:Y20">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="formula" val="0%"/>
@@ -1830,17 +2530,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I20 K3:K20 M3:M20 O3:O20 Q3:Q20">
+  <conditionalFormatting sqref="I3:I20 K3:K20 M3:M20 O3:O20 Q3:Q20 S3:S20 U3:U20 W3:W20 Y3:Y20">
     <cfRule type="containsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(I3))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J20 L3:L20 N3:N20 P3:P20 R3:R20">
+  <conditionalFormatting sqref="J3:J20 L3:L20 N3:N20 P3:P20 R3:R20 T3:T20 V3:V20 X3:X20 Z3:AB20 I22 K22 M22 O22 Q22 S22 U22 W22 Y22">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J20 L3:L20 N3:N20 P3:P20 R3:R20">
+  <conditionalFormatting sqref="J3:J20 L3:L20 N3:N20 P3:P20 R3:R20 T3:T20 V3:V20 X3:X20 Z3:AB20 I22 K22 M22 O22 Q22 S22 U22 W22 Y22">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="formula" val="0"/>

</xml_diff>